<commit_message>
Add more training datas.
</commit_message>
<xml_diff>
--- a/analyse/训练记录-autd.xlsx
+++ b/analyse/训练记录-autd.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="286">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1075,6 +1075,25 @@
   </si>
   <si>
     <t>经过约6小时，拟合精度还能提高，泛化精度难再提高了，慢慢分化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_size=100 low_nums=5 use_biases=yes use_bn_low=True dropout_low=0.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高标签，重新训练，PCA及Wavelet处理数据train-hjxh365-2018-4-16-day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python feed_run.py --output_mode=classes --output_nodes=14 --input_nums=39 --input_nodes=39 --low_nums=5 --low_nodes=39 --low_fun=elu --use_bn_input=True --one_hot=True --input_fun=tanh --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5400 --test_size=1339 --use_biases=yes --dropout_low=0.8</t>
+  </si>
+  <si>
+    <t>logs-hjxh-2018-4-23-class14-pca99-wavelet20-percent65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过约82小时，拟合精度还能提高，泛化精度看来还可以再提高一点，不过慢</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1457,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3986,6 +4005,44 @@
       </c>
       <c r="L68" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="82.5" customHeight="1">
+      <c r="A69" s="6">
+        <v>43213.034722222219</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L69" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New datas with more features.
</commit_message>
<xml_diff>
--- a/analyse/训练记录-autd.xlsx
+++ b/analyse/训练记录-autd.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="294">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1109,6 +1109,20 @@
   </si>
   <si>
     <t>logs-hjxh365-4-23-high-norm-pca99-vavelet20-percent64</t>
+  </si>
+  <si>
+    <t>最高标签，重新训练，原始数据加上序列train-hjxh365-2018-4-16-day-high-sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python feed_run.py --output_mode=classes --output_nodes=14 --input_nums=129 --input_nodes=129 --low_nums=2 --low_nodes=129 --low_fun=elu --use_bn_input=True --one_hot=True --input_fun=tanh --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5400 --test_size=1339 --use_biases=yes --dropout_low=0.7</t>
+  </si>
+  <si>
+    <t>logs-hjxh-2018-4-24-class14-sequence-percent60</t>
+  </si>
+  <si>
+    <t>经过约17小时，拟合精度还能提高，泛化精度无法提高了，还有点下降，两者已明显分化。看来加入单纯序列不利于泛化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1490,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4095,6 +4109,44 @@
       </c>
       <c r="L70" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="82.5" customHeight="1">
+      <c r="A71" s="6">
+        <v>43214.347222222219</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="L71" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new training datas.
</commit_message>
<xml_diff>
--- a/analyse/训练记录-autd.xlsx
+++ b/analyse/训练记录-autd.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="319">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1201,6 +1201,21 @@
   </si>
   <si>
     <t>python3 feed_run.py --output_mode=classes --output_nodes=14 --input_nums=39 --input_nodes=39 --low_nums=3 --low_nodes=39 --low_fun=elu --one_hot=True --input_fun=elu --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5400 --test_size=1339 --use_biases=yes</t>
+  </si>
+  <si>
+    <t>logs-hjxh-2018-4-27-class14-original-more-percent64</t>
+  </si>
+  <si>
+    <t>python feed_run.py --output_mode=classes --output_nodes=14 --input_nums=92 --input_nodes=92 --low_nums=2 --low_nodes=92 --low_fun=elu --one_hot=True --input_fun=tanh --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5400 --test_size=1339 --use_biases=yes --dropout_in=0.6 --dropout_low=0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_size=100 low_nums=2 use_biases=yes  dropout_in=0.6  dropout_low=0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过约41小时，拟合精度和泛化精度接近，运行较久，但是没多少变化和进展。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1582,9 +1597,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D76" workbookViewId="0">
       <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
@@ -4415,6 +4430,44 @@
       </c>
       <c r="L76" t="s">
         <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="82.5" customHeight="1">
+      <c r="A77" s="6">
+        <v>43217.356944444444</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="L77" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new record information.
</commit_message>
<xml_diff>
--- a/analyse/训练记录-autd.xlsx
+++ b/analyse/训练记录-autd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="456">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1713,6 +1713,25 @@
   </si>
   <si>
     <t>logs-hjxh-2018-5-16-high-check-percent61</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高标签，重新训练，新加指标未归一化数据,删除前面不规则数据train-hjxh365-2018-4-16-day-high-check-clear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过约8小时，精度分化较早.波动不大，最好达到0.63，比没删除数据好像要好点。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logs-hjxh-2018-5-16-high-check-clear-percent62</t>
+  </si>
+  <si>
+    <t>python feed_run.py --output_mode=classes --output_nodes=14 --input_nums=90 --input_nodes=90 --low_nums=2 --low_nodes=90 --low_fun=elu --one_hot=True --input_fun=tanh  --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5400 --test_size=1280 --use_biases=yes  --use_bn_low=True  --dropout_low=0.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_size=100 low_nums=2 use_biases=yes dropout_low=0.8 use_bn_low=True</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2095,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6182,6 +6201,44 @@
       </c>
       <c r="L109" t="s">
         <v>450</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="82.5" customHeight="1">
+      <c r="A110" s="6">
+        <v>43236.75</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="K110" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="L110" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add codes and record.
</commit_message>
<xml_diff>
--- a/analyse/训练记录-autd.xlsx
+++ b/analyse/训练记录-autd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="670">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2485,6 +2485,28 @@
   </si>
   <si>
     <t>logs-hjxh-2018-7-15-low-ori-trim4-percent63</t>
+  </si>
+  <si>
+    <t>11分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size=100 low_nums=2 use_biases=yes use_bn_input=True </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高标签，重新训练train-365-hjxh-2018-7-23-day-hima-ori20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过约39小时，拟合在泛化之上，泛化最好为0.66。后面慢慢分化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python feed_run.py --output_mode=classes --output_nodes=11 --input_nums=20 --input_nodes=20 --low_nums=2 --low_nodes=20 --low_fun=elu --one_hot=True --input_fun=tanh  --batch_size=100 --learning_rate=0.001 --train_mode=Adadelta --eval_size=5450 --test_size=1359 --use_biases=yes --use_bn_input=True</t>
+  </si>
+  <si>
+    <t>logs-hjxh-2018-7-25-day-hima-ori20-percent64</t>
   </si>
 </sst>
 </file>
@@ -2914,10 +2936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L166"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="K164" workbookViewId="0">
+      <selection activeCell="L167" sqref="L167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9167,6 +9189,44 @@
       </c>
       <c r="L166" s="19" t="s">
         <v>663</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" s="19" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A167" s="16">
+        <v>43306.354166666664</v>
+      </c>
+      <c r="B167" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="C167" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="D167" s="17" t="s">
+        <v>665</v>
+      </c>
+      <c r="E167" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="F167" s="17">
+        <v>0.64</v>
+      </c>
+      <c r="G167" s="17">
+        <v>0.64</v>
+      </c>
+      <c r="H167" s="17">
+        <v>1</v>
+      </c>
+      <c r="I167" s="17">
+        <v>0.99</v>
+      </c>
+      <c r="J167" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="K167" s="18" t="s">
+        <v>668</v>
+      </c>
+      <c r="L167" s="19" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>